<commit_message>
add 'How to use' section in Excel
</commit_message>
<xml_diff>
--- a/planning/Excels/Templates/AOBNOBAMXCMX_template.xlsx
+++ b/planning/Excels/Templates/AOBNOBAMXCMX_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Google Drive\Uni\Master Thesis\version_GitHub\planning\Excels\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF44AE01-3792-45C9-8075-BBC33CB19485}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1ABA3FB-8D87-4BE8-A46E-47E792489387}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" tabRatio="808" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" tabRatio="808" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Information" sheetId="30" r:id="rId1"/>
@@ -171,7 +171,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="547" uniqueCount="269">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="556" uniqueCount="278">
   <si>
     <t>AOB/AOA</t>
   </si>
@@ -1410,6 +1410,33 @@
   <si>
     <t>Compound name for which the concentration should be below given threshold (i.e. Setpoint). Make sure this name matches the compound name in rest of the Excel file</t>
   </si>
+  <si>
+    <t>How to use this Excel sheet</t>
+  </si>
+  <si>
+    <t>All values in this file are loaded into the IbM model using the loadPresetFile function. Make sure that all values are filled in correctly, so that the model makes sense.</t>
+  </si>
+  <si>
+    <t>There are a few different types of cells in this Excel, here is a legend:</t>
+  </si>
+  <si>
+    <t>Cells that look like this, contain calculated values, don't change these.</t>
+  </si>
+  <si>
+    <t>This cell contains the name of the variable/short description</t>
+  </si>
+  <si>
+    <t>This cell contains a value that has been manually adjusted (Make sure to mark these cells yourself, so that it is clear later on which values are changed from the standard calculation/value)</t>
+  </si>
+  <si>
+    <t>Fill in all cells that look like this</t>
+  </si>
+  <si>
+    <t>Due to some setting, some cells no longer need to be filled in. If that is the case, those cells look like this</t>
+  </si>
+  <si>
+    <t>This cell contains the units of the value that should be filled in. Don’t change the contents of these cells, but rather make sure that the filled in value is in these units</t>
+  </si>
 </sst>
 </file>
 
@@ -1425,7 +1452,7 @@
     <numFmt numFmtId="170" formatCode="0.0"/>
     <numFmt numFmtId="171" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="42" x14ac:knownFonts="1">
+  <fonts count="43" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1693,6 +1720,13 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="16"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="13">
     <fill>
@@ -2844,7 +2878,7 @@
     <xf numFmtId="0" fontId="35" fillId="11" borderId="39" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="37" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="247">
+  <cellXfs count="256">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="7"/>
     <xf numFmtId="169" fontId="1" fillId="0" borderId="0" xfId="7" applyNumberFormat="1"/>
@@ -3495,6 +3529,31 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="50" xfId="10" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="10" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="37" fillId="0" borderId="35" xfId="11" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="11" fontId="41" fillId="12" borderId="35" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="11" borderId="36" xfId="10" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="34" xfId="10" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="12">
@@ -3511,7 +3570,7 @@
     <cellStyle name="Percent" xfId="8" builtinId="5"/>
     <cellStyle name="Warning Text" xfId="9" builtinId="11"/>
   </cellStyles>
-  <dxfs count="88">
+  <dxfs count="93">
     <dxf>
       <font>
         <color theme="0" tint="-0.24994659260841701"/>
@@ -3899,6 +3958,16 @@
     </dxf>
     <dxf>
       <font>
+        <color theme="0" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <strike val="0"/>
         <color theme="0" tint="-0.24994659260841701"/>
       </font>
@@ -3986,6 +4055,37 @@
     <dxf>
       <font>
         <color theme="0" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+        <color theme="0" tint="-0.34998626667073579"/>
       </font>
     </dxf>
     <dxf>
@@ -4366,10 +4466,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6616838C-F568-417D-8029-DEFF7E533FF8}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -4411,8 +4511,77 @@
         <v>116</v>
       </c>
     </row>
+    <row r="9" spans="1:3" ht="21" x14ac:dyDescent="0.4">
+      <c r="A9" s="254" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
+      <c r="A10" s="255" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="253" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="252" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="28.8" x14ac:dyDescent="0.25">
+      <c r="A13" s="248" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A14" s="247" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
+      <c r="A15" s="249" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
+      <c r="A16" s="250" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="251" t="s">
+        <v>276</v>
+      </c>
+    </row>
   </sheetData>
+  <conditionalFormatting sqref="A15">
+    <cfRule type="expression" dxfId="90" priority="6">
+      <formula>$B$2 = FALSE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A16">
+    <cfRule type="containsText" dxfId="89" priority="4" operator="containsText" text="NA">
+      <formula>NOT(ISERROR(SEARCH("NA",A16)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="88" priority="5" operator="containsText" text="Inf">
+      <formula>NOT(ISERROR(SEARCH("Inf",A16)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A16">
+    <cfRule type="cellIs" dxfId="87" priority="3" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A17">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>$B$11&lt;&gt;"naive"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -4576,7 +4745,7 @@
   <dimension ref="A1:I33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -9304,82 +9473,82 @@
     <mergeCell ref="N27:Q27"/>
   </mergeCells>
   <conditionalFormatting sqref="S5:AB7 AD5:AD7 AD9:AD16 S9:AB16">
-    <cfRule type="cellIs" dxfId="84" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="85" priority="18" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S17:AD23">
-    <cfRule type="cellIs" dxfId="83" priority="19" operator="notBetween">
+    <cfRule type="cellIs" dxfId="84" priority="19" operator="notBetween">
       <formula>0.0000000001</formula>
       <formula>-0.0000000001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="82" priority="20" operator="between">
+    <cfRule type="cellIs" dxfId="83" priority="20" operator="between">
       <formula>0.0000000001</formula>
       <formula>-0.0000000001</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S8:AB8 AD8">
-    <cfRule type="cellIs" dxfId="81" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="82" priority="13" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC5:AC7 AC9:AC16">
-    <cfRule type="cellIs" dxfId="80" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="81" priority="12" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC8">
-    <cfRule type="cellIs" dxfId="79" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="80" priority="11" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG8">
-    <cfRule type="cellIs" dxfId="78" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="79" priority="5" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AE5:AF7 AE9:AF16 AH9:AI16 AH5:AJ5 AH6:AI7 AJ6:AJ16 AH4">
-    <cfRule type="cellIs" dxfId="77" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="78" priority="8" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AE17:AJ23">
-    <cfRule type="cellIs" dxfId="76" priority="9" operator="notBetween">
+    <cfRule type="cellIs" dxfId="77" priority="9" operator="notBetween">
       <formula>0.0000000001</formula>
       <formula>-0.0000000001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="75" priority="10" operator="between">
+    <cfRule type="cellIs" dxfId="76" priority="10" operator="between">
       <formula>0.0000000001</formula>
       <formula>-0.0000000001</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AE8:AF8 AH8:AI8">
-    <cfRule type="cellIs" dxfId="74" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="75" priority="7" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG5:AG7 AG9:AG16">
-    <cfRule type="cellIs" dxfId="73" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="74" priority="6" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD4 S4:AB4">
-    <cfRule type="cellIs" dxfId="72" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="73" priority="4" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC4">
-    <cfRule type="cellIs" dxfId="71" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="72" priority="3" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AE4:AF4 AI4">
-    <cfRule type="cellIs" dxfId="70" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="71" priority="2" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG4">
-    <cfRule type="cellIs" dxfId="69" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="70" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9392,9 +9561,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CC80DB5-92D9-44E1-984F-05E418326CA4}">
   <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
@@ -9531,7 +9698,7 @@
   <dimension ref="A1:E28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -9983,7 +10150,7 @@
     <mergeCell ref="E15:E28"/>
   </mergeCells>
   <conditionalFormatting sqref="A16:D28">
-    <cfRule type="expression" dxfId="68" priority="1">
+    <cfRule type="expression" dxfId="69" priority="1">
       <formula>$B$15 = FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10001,8 +10168,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:E29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -10268,12 +10435,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A3:D4">
-    <cfRule type="expression" dxfId="67" priority="3">
+    <cfRule type="expression" dxfId="68" priority="3">
       <formula>$B$2 = FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:D1">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="67" priority="1">
       <formula>$B$2=TRUE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10435,7 +10602,7 @@
   <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>

</xml_diff>